<commit_message>
Enseñando a usar cmd
</commit_message>
<xml_diff>
--- a/Cálculos del Proyecto de AEEE.xlsx
+++ b/Cálculos del Proyecto de AEEE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdavi\Desktop\Proyecto AEE\ProyectoFinalAEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3613AE9F-6F87-4E0E-B377-71CE08221977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277CB672-E48A-42A1-A531-D1F76E6A85FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11310" tabRatio="814" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -743,7 +743,7 @@
     <t>(-) Impuestos 9%</t>
   </si>
   <si>
-    <t>Que ondas mariella</t>
+    <t xml:space="preserve">Que ondas mariella </t>
   </si>
 </sst>
 </file>
@@ -2486,6 +2486,81 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="21" borderId="62" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="21" borderId="63" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="21" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2528,153 +2603,78 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="21" borderId="62" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="21" borderId="63" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="21" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2692,36 +2692,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="5" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="13" fillId="14" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="13" fillId="14" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2735,6 +2705,36 @@
     </xf>
     <xf numFmtId="169" fontId="13" fillId="15" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="5" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="14" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="14" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -6062,49 +6062,49 @@
   <sheetData>
     <row r="1" spans="2:14" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="207" t="s">
+      <c r="B2" s="194" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
-      <c r="H2" s="208"/>
-      <c r="I2" s="208"/>
-      <c r="J2" s="208"/>
-      <c r="K2" s="208"/>
-      <c r="L2" s="208"/>
-      <c r="M2" s="208"/>
-      <c r="N2" s="209"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="195"/>
+      <c r="L2" s="195"/>
+      <c r="M2" s="195"/>
+      <c r="N2" s="196"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="210" t="s">
+      <c r="B3" s="197" t="s">
         <v>187</v>
       </c>
-      <c r="C3" s="211"/>
-      <c r="D3" s="212"/>
-      <c r="E3" s="204" t="s">
+      <c r="C3" s="198"/>
+      <c r="D3" s="199"/>
+      <c r="E3" s="191" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="205"/>
-      <c r="G3" s="204"/>
-      <c r="H3" s="204"/>
-      <c r="I3" s="204"/>
-      <c r="J3" s="204"/>
-      <c r="K3" s="204"/>
-      <c r="L3" s="204"/>
-      <c r="M3" s="204"/>
-      <c r="N3" s="206"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="191"/>
+      <c r="H3" s="191"/>
+      <c r="I3" s="191"/>
+      <c r="J3" s="191"/>
+      <c r="K3" s="191"/>
+      <c r="L3" s="191"/>
+      <c r="M3" s="191"/>
+      <c r="N3" s="193"/>
     </row>
     <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="213"/>
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
-      <c r="E4" s="217">
+      <c r="B4" s="200"/>
+      <c r="C4" s="201"/>
+      <c r="D4" s="201"/>
+      <c r="E4" s="204">
         <v>1</v>
       </c>
-      <c r="F4" s="220">
+      <c r="F4" s="207">
         <v>2</v>
       </c>
       <c r="G4" s="184">
@@ -6133,15 +6133,15 @@
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="223" t="s">
+      <c r="B5" s="210" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="224"/>
-      <c r="D5" s="215" t="s">
+      <c r="C5" s="211"/>
+      <c r="D5" s="202" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="218"/>
-      <c r="F5" s="221"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="208"/>
       <c r="G5" s="185"/>
       <c r="H5" s="185"/>
       <c r="I5" s="185"/>
@@ -6158,9 +6158,9 @@
       <c r="C6" s="142" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="216"/>
-      <c r="E6" s="219"/>
-      <c r="F6" s="222"/>
+      <c r="D6" s="203"/>
+      <c r="E6" s="206"/>
+      <c r="F6" s="209"/>
       <c r="G6" s="186"/>
       <c r="H6" s="186"/>
       <c r="I6" s="186"/>
@@ -6177,7 +6177,7 @@
       <c r="C7" s="138" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="201">
+      <c r="D7" s="188">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E7" s="143">
@@ -6227,7 +6227,7 @@
       <c r="C8" s="138" t="s">
         <v>135</v>
       </c>
-      <c r="D8" s="202"/>
+      <c r="D8" s="189"/>
       <c r="E8" s="145">
         <v>56</v>
       </c>
@@ -6275,7 +6275,7 @@
       <c r="C9" s="138" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="202"/>
+      <c r="D9" s="189"/>
       <c r="E9" s="145">
         <v>84</v>
       </c>
@@ -6323,7 +6323,7 @@
       <c r="C10" s="138" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="202"/>
+      <c r="D10" s="189"/>
       <c r="E10" s="145">
         <v>23</v>
       </c>
@@ -6371,7 +6371,7 @@
       <c r="C11" s="138" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="202"/>
+      <c r="D11" s="189"/>
       <c r="E11" s="145">
         <v>16</v>
       </c>
@@ -6419,7 +6419,7 @@
       <c r="C12" s="138" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="202"/>
+      <c r="D12" s="189"/>
       <c r="E12" s="145">
         <v>14</v>
       </c>
@@ -6467,7 +6467,7 @@
       <c r="C13" s="138" t="s">
         <v>140</v>
       </c>
-      <c r="D13" s="202"/>
+      <c r="D13" s="189"/>
       <c r="E13" s="145">
         <v>35</v>
       </c>
@@ -6515,7 +6515,7 @@
       <c r="C14" s="138" t="s">
         <v>141</v>
       </c>
-      <c r="D14" s="202"/>
+      <c r="D14" s="189"/>
       <c r="E14" s="145">
         <v>14</v>
       </c>
@@ -6563,7 +6563,7 @@
       <c r="C15" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="D15" s="202"/>
+      <c r="D15" s="189"/>
       <c r="E15" s="145">
         <v>7.5</v>
       </c>
@@ -6611,7 +6611,7 @@
       <c r="C16" s="138" t="s">
         <v>143</v>
       </c>
-      <c r="D16" s="202"/>
+      <c r="D16" s="189"/>
       <c r="E16" s="145">
         <v>5</v>
       </c>
@@ -6659,7 +6659,7 @@
       <c r="C17" s="138" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="202"/>
+      <c r="D17" s="189"/>
       <c r="E17" s="145">
         <v>3.75</v>
       </c>
@@ -6707,7 +6707,7 @@
       <c r="C18" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="D18" s="202"/>
+      <c r="D18" s="189"/>
       <c r="E18" s="145">
         <v>10</v>
       </c>
@@ -6755,7 +6755,7 @@
       <c r="C19" s="138" t="s">
         <v>144</v>
       </c>
-      <c r="D19" s="202"/>
+      <c r="D19" s="189"/>
       <c r="E19" s="145">
         <v>28</v>
       </c>
@@ -6803,7 +6803,7 @@
       <c r="C20" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="D20" s="202"/>
+      <c r="D20" s="189"/>
       <c r="E20" s="145">
         <v>25</v>
       </c>
@@ -6851,7 +6851,7 @@
       <c r="C21" s="138" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="202"/>
+      <c r="D21" s="189"/>
       <c r="E21" s="145">
         <v>6.3</v>
       </c>
@@ -6899,7 +6899,7 @@
       <c r="C22" s="138" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="202"/>
+      <c r="D22" s="189"/>
       <c r="E22" s="145">
         <v>227.5</v>
       </c>
@@ -6947,7 +6947,7 @@
       <c r="C23" s="138" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="202"/>
+      <c r="D23" s="189"/>
       <c r="E23" s="145">
         <v>70</v>
       </c>
@@ -6995,7 +6995,7 @@
       <c r="C24" s="138" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="202"/>
+      <c r="D24" s="189"/>
       <c r="E24" s="145">
         <v>30.5</v>
       </c>
@@ -7043,7 +7043,7 @@
       <c r="C25" s="138" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="202"/>
+      <c r="D25" s="189"/>
       <c r="E25" s="145">
         <v>85.5</v>
       </c>
@@ -7091,7 +7091,7 @@
       <c r="C26" s="138" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="202"/>
+      <c r="D26" s="189"/>
       <c r="E26" s="145">
         <v>175</v>
       </c>
@@ -7139,7 +7139,7 @@
       <c r="C27" s="138" t="s">
         <v>148</v>
       </c>
-      <c r="D27" s="202"/>
+      <c r="D27" s="189"/>
       <c r="E27" s="145">
         <v>31.5</v>
       </c>
@@ -7187,7 +7187,7 @@
       <c r="C28" s="138" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="202"/>
+      <c r="D28" s="189"/>
       <c r="E28" s="147">
         <v>141.75</v>
       </c>
@@ -7235,7 +7235,7 @@
       <c r="C29" s="140" t="s">
         <v>146</v>
       </c>
-      <c r="D29" s="202"/>
+      <c r="D29" s="189"/>
       <c r="E29" s="147">
         <v>80.5</v>
       </c>
@@ -7283,7 +7283,7 @@
       <c r="C30" s="140" t="s">
         <v>152</v>
       </c>
-      <c r="D30" s="202"/>
+      <c r="D30" s="189"/>
       <c r="E30" s="147">
         <f>702/52</f>
         <v>13.5</v>
@@ -7332,7 +7332,7 @@
       <c r="C31" s="140" t="s">
         <v>153</v>
       </c>
-      <c r="D31" s="202"/>
+      <c r="D31" s="189"/>
       <c r="E31" s="147">
         <v>28.56</v>
       </c>
@@ -7380,7 +7380,7 @@
       <c r="C32" s="140" t="s">
         <v>154</v>
       </c>
-      <c r="D32" s="202"/>
+      <c r="D32" s="189"/>
       <c r="E32" s="147">
         <v>7</v>
       </c>
@@ -7428,7 +7428,7 @@
       <c r="C33" s="140" t="s">
         <v>155</v>
       </c>
-      <c r="D33" s="202"/>
+      <c r="D33" s="189"/>
       <c r="E33" s="147">
         <v>15</v>
       </c>
@@ -7476,7 +7476,7 @@
       <c r="C34" s="140" t="s">
         <v>156</v>
       </c>
-      <c r="D34" s="202"/>
+      <c r="D34" s="189"/>
       <c r="E34" s="147">
         <v>20.58</v>
       </c>
@@ -7524,7 +7524,7 @@
       <c r="C35" s="140" t="s">
         <v>157</v>
       </c>
-      <c r="D35" s="202"/>
+      <c r="D35" s="189"/>
       <c r="E35" s="147">
         <v>22.72</v>
       </c>
@@ -7572,7 +7572,7 @@
       <c r="C36" s="140" t="s">
         <v>158</v>
       </c>
-      <c r="D36" s="202"/>
+      <c r="D36" s="189"/>
       <c r="E36" s="147">
         <v>8</v>
       </c>
@@ -7620,7 +7620,7 @@
       <c r="C37" s="140" t="s">
         <v>158</v>
       </c>
-      <c r="D37" s="202"/>
+      <c r="D37" s="189"/>
       <c r="E37" s="147">
         <v>8</v>
       </c>
@@ -7668,7 +7668,7 @@
       <c r="C38" s="140" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="202"/>
+      <c r="D38" s="189"/>
       <c r="E38" s="147">
         <v>11.25</v>
       </c>
@@ -7716,7 +7716,7 @@
       <c r="C39" s="140" t="s">
         <v>159</v>
       </c>
-      <c r="D39" s="202"/>
+      <c r="D39" s="189"/>
       <c r="E39" s="147">
         <v>12.5</v>
       </c>
@@ -7764,7 +7764,7 @@
       <c r="C40" s="140" t="s">
         <v>160</v>
       </c>
-      <c r="D40" s="202"/>
+      <c r="D40" s="189"/>
       <c r="E40" s="147">
         <v>12</v>
       </c>
@@ -7812,7 +7812,7 @@
       <c r="C41" s="140" t="s">
         <v>143</v>
       </c>
-      <c r="D41" s="202"/>
+      <c r="D41" s="189"/>
       <c r="E41" s="147">
         <v>10</v>
       </c>
@@ -7860,7 +7860,7 @@
       <c r="C42" s="140" t="s">
         <v>161</v>
       </c>
-      <c r="D42" s="202"/>
+      <c r="D42" s="189"/>
       <c r="E42" s="147">
         <v>120</v>
       </c>
@@ -7908,7 +7908,7 @@
       <c r="C43" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D43" s="202"/>
+      <c r="D43" s="189"/>
       <c r="E43" s="147">
         <v>66</v>
       </c>
@@ -7956,7 +7956,7 @@
       <c r="C44" s="140" t="s">
         <v>163</v>
       </c>
-      <c r="D44" s="202"/>
+      <c r="D44" s="189"/>
       <c r="E44" s="147">
         <v>7</v>
       </c>
@@ -8004,7 +8004,7 @@
       <c r="C45" s="140" t="s">
         <v>178</v>
       </c>
-      <c r="D45" s="202"/>
+      <c r="D45" s="189"/>
       <c r="E45" s="147">
         <v>2.72</v>
       </c>
@@ -8052,7 +8052,7 @@
       <c r="C46" s="140" t="s">
         <v>164</v>
       </c>
-      <c r="D46" s="202"/>
+      <c r="D46" s="189"/>
       <c r="E46" s="147">
         <v>3.6</v>
       </c>
@@ -8100,7 +8100,7 @@
       <c r="C47" s="140" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="202"/>
+      <c r="D47" s="189"/>
       <c r="E47" s="147">
         <v>4.25</v>
       </c>
@@ -8148,7 +8148,7 @@
       <c r="C48" s="140" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="202"/>
+      <c r="D48" s="189"/>
       <c r="E48" s="147">
         <v>4.25</v>
       </c>
@@ -8196,7 +8196,7 @@
       <c r="C49" s="140" t="s">
         <v>166</v>
       </c>
-      <c r="D49" s="202"/>
+      <c r="D49" s="189"/>
       <c r="E49" s="147">
         <v>6</v>
       </c>
@@ -8244,7 +8244,7 @@
       <c r="C50" s="140" t="s">
         <v>164</v>
       </c>
-      <c r="D50" s="202"/>
+      <c r="D50" s="189"/>
       <c r="E50" s="147">
         <v>9</v>
       </c>
@@ -8292,7 +8292,7 @@
       <c r="C51" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="D51" s="202"/>
+      <c r="D51" s="189"/>
       <c r="E51" s="147">
         <v>7</v>
       </c>
@@ -8340,7 +8340,7 @@
       <c r="C52" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="D52" s="202"/>
+      <c r="D52" s="189"/>
       <c r="E52" s="147">
         <v>8</v>
       </c>
@@ -8388,7 +8388,7 @@
       <c r="C53" s="140" t="s">
         <v>148</v>
       </c>
-      <c r="D53" s="202"/>
+      <c r="D53" s="189"/>
       <c r="E53" s="147">
         <v>10</v>
       </c>
@@ -8436,7 +8436,7 @@
       <c r="C54" s="140" t="s">
         <v>168</v>
       </c>
-      <c r="D54" s="202"/>
+      <c r="D54" s="189"/>
       <c r="E54" s="147">
         <v>4.9000000000000004</v>
       </c>
@@ -8484,7 +8484,7 @@
       <c r="C55" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="D55" s="202"/>
+      <c r="D55" s="189"/>
       <c r="E55" s="147">
         <v>18</v>
       </c>
@@ -8532,7 +8532,7 @@
       <c r="C56" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="D56" s="202"/>
+      <c r="D56" s="189"/>
       <c r="E56" s="147">
         <v>10</v>
       </c>
@@ -8580,7 +8580,7 @@
       <c r="C57" s="140" t="s">
         <v>171</v>
       </c>
-      <c r="D57" s="202"/>
+      <c r="D57" s="189"/>
       <c r="E57" s="147">
         <v>7</v>
       </c>
@@ -8628,7 +8628,7 @@
       <c r="C58" s="140" t="s">
         <v>172</v>
       </c>
-      <c r="D58" s="202"/>
+      <c r="D58" s="189"/>
       <c r="E58" s="147">
         <v>1.58</v>
       </c>
@@ -8676,7 +8676,7 @@
       <c r="C59" s="140" t="s">
         <v>173</v>
       </c>
-      <c r="D59" s="202"/>
+      <c r="D59" s="189"/>
       <c r="E59" s="147">
         <v>19</v>
       </c>
@@ -8724,7 +8724,7 @@
       <c r="C60" s="140" t="s">
         <v>174</v>
       </c>
-      <c r="D60" s="202"/>
+      <c r="D60" s="189"/>
       <c r="E60" s="147">
         <v>5.4</v>
       </c>
@@ -8772,7 +8772,7 @@
       <c r="C61" s="140" t="s">
         <v>175</v>
       </c>
-      <c r="D61" s="202"/>
+      <c r="D61" s="189"/>
       <c r="E61" s="147">
         <v>6.25</v>
       </c>
@@ -8820,7 +8820,7 @@
       <c r="C62" s="140" t="s">
         <v>176</v>
       </c>
-      <c r="D62" s="202"/>
+      <c r="D62" s="189"/>
       <c r="E62" s="147">
         <v>4.5</v>
       </c>
@@ -8868,7 +8868,7 @@
       <c r="C63" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="D63" s="202"/>
+      <c r="D63" s="189"/>
       <c r="E63" s="149">
         <v>42</v>
       </c>
@@ -8916,7 +8916,7 @@
       <c r="C64" s="140" t="s">
         <v>211</v>
       </c>
-      <c r="D64" s="202"/>
+      <c r="D64" s="189"/>
       <c r="E64" s="166">
         <v>15.2</v>
       </c>
@@ -8964,7 +8964,7 @@
       <c r="C65" s="140" t="s">
         <v>212</v>
       </c>
-      <c r="D65" s="202"/>
+      <c r="D65" s="189"/>
       <c r="E65" s="166">
         <v>6.96</v>
       </c>
@@ -9012,7 +9012,7 @@
       <c r="C66" s="140" t="s">
         <v>213</v>
       </c>
-      <c r="D66" s="202"/>
+      <c r="D66" s="189"/>
       <c r="E66" s="166">
         <v>16.32</v>
       </c>
@@ -9060,7 +9060,7 @@
       <c r="C67" s="140" t="s">
         <v>213</v>
       </c>
-      <c r="D67" s="202"/>
+      <c r="D67" s="189"/>
       <c r="E67" s="166">
         <v>16.32</v>
       </c>
@@ -9108,7 +9108,7 @@
       <c r="C68" s="140" t="s">
         <v>214</v>
       </c>
-      <c r="D68" s="202"/>
+      <c r="D68" s="189"/>
       <c r="E68" s="166">
         <v>5.5</v>
       </c>
@@ -9156,7 +9156,7 @@
       <c r="C69" s="140" t="s">
         <v>215</v>
       </c>
-      <c r="D69" s="202"/>
+      <c r="D69" s="189"/>
       <c r="E69" s="166">
         <v>13</v>
       </c>
@@ -9204,7 +9204,7 @@
       <c r="C70" s="140" t="s">
         <v>216</v>
       </c>
-      <c r="D70" s="202"/>
+      <c r="D70" s="189"/>
       <c r="E70" s="166">
         <v>141.12</v>
       </c>
@@ -9252,7 +9252,7 @@
       <c r="C71" s="140" t="s">
         <v>217</v>
       </c>
-      <c r="D71" s="202"/>
+      <c r="D71" s="189"/>
       <c r="E71" s="166">
         <v>15.68</v>
       </c>
@@ -9300,7 +9300,7 @@
       <c r="C72" s="140" t="s">
         <v>226</v>
       </c>
-      <c r="D72" s="202"/>
+      <c r="D72" s="189"/>
       <c r="E72" s="165">
         <v>54.6</v>
       </c>
@@ -9348,7 +9348,7 @@
       <c r="C73" s="140" t="s">
         <v>227</v>
       </c>
-      <c r="D73" s="202"/>
+      <c r="D73" s="189"/>
       <c r="E73" s="165">
         <v>11</v>
       </c>
@@ -9396,7 +9396,7 @@
       <c r="C74" s="140" t="s">
         <v>228</v>
       </c>
-      <c r="D74" s="202"/>
+      <c r="D74" s="189"/>
       <c r="E74" s="165">
         <v>56.1</v>
       </c>
@@ -9444,7 +9444,7 @@
       <c r="C75" s="140" t="s">
         <v>229</v>
       </c>
-      <c r="D75" s="202"/>
+      <c r="D75" s="189"/>
       <c r="E75" s="165">
         <v>15</v>
       </c>
@@ -9492,7 +9492,7 @@
       <c r="C76" s="140" t="s">
         <v>230</v>
       </c>
-      <c r="D76" s="202"/>
+      <c r="D76" s="189"/>
       <c r="E76" s="165">
         <v>90</v>
       </c>
@@ -9540,7 +9540,7 @@
       <c r="C77" s="140" t="s">
         <v>231</v>
       </c>
-      <c r="D77" s="202"/>
+      <c r="D77" s="189"/>
       <c r="E77" s="165">
         <v>4</v>
       </c>
@@ -9588,7 +9588,7 @@
       <c r="C78" s="140" t="s">
         <v>232</v>
       </c>
-      <c r="D78" s="202"/>
+      <c r="D78" s="189"/>
       <c r="E78" s="165">
         <v>4.0999999999999996</v>
       </c>
@@ -9636,7 +9636,7 @@
       <c r="C79" s="140" t="s">
         <v>233</v>
       </c>
-      <c r="D79" s="203"/>
+      <c r="D79" s="190"/>
       <c r="E79" s="165">
         <v>7</v>
       </c>
@@ -9678,10 +9678,10 @@
       </c>
     </row>
     <row r="80" spans="2:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="200" t="s">
+      <c r="B80" s="187" t="s">
         <v>188</v>
       </c>
-      <c r="C80" s="200"/>
+      <c r="C80" s="187"/>
       <c r="D80" s="176"/>
       <c r="E80" s="171">
         <f>SUM(E7:E79)*26</f>
@@ -9725,11 +9725,11 @@
       </c>
     </row>
     <row r="81" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="193" t="s">
+      <c r="B81" s="218" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="194"/>
-      <c r="D81" s="195"/>
+      <c r="C81" s="219"/>
+      <c r="D81" s="220"/>
       <c r="E81" s="172"/>
       <c r="F81" s="172"/>
       <c r="G81" s="172"/>
@@ -9742,11 +9742,11 @@
       <c r="N81" s="173"/>
     </row>
     <row r="82" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="196" t="s">
+      <c r="B82" s="221" t="s">
         <v>67</v>
       </c>
-      <c r="C82" s="197"/>
-      <c r="D82" s="198"/>
+      <c r="C82" s="222"/>
+      <c r="D82" s="223"/>
       <c r="E82" s="108">
         <v>300</v>
       </c>
@@ -9779,11 +9779,11 @@
       </c>
     </row>
     <row r="83" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="196" t="s">
+      <c r="B83" s="221" t="s">
         <v>68</v>
       </c>
-      <c r="C83" s="197"/>
-      <c r="D83" s="198"/>
+      <c r="C83" s="222"/>
+      <c r="D83" s="223"/>
       <c r="E83" s="108">
         <v>1100</v>
       </c>
@@ -9816,11 +9816,11 @@
       </c>
     </row>
     <row r="84" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="196" t="s">
+      <c r="B84" s="221" t="s">
         <v>69</v>
       </c>
-      <c r="C84" s="197"/>
-      <c r="D84" s="198"/>
+      <c r="C84" s="222"/>
+      <c r="D84" s="223"/>
       <c r="E84" s="108">
         <v>400</v>
       </c>
@@ -9853,11 +9853,11 @@
       </c>
     </row>
     <row r="85" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="196" t="s">
+      <c r="B85" s="221" t="s">
         <v>185</v>
       </c>
-      <c r="C85" s="197"/>
-      <c r="D85" s="198"/>
+      <c r="C85" s="222"/>
+      <c r="D85" s="223"/>
       <c r="E85" s="108">
         <v>1920</v>
       </c>
@@ -9890,11 +9890,11 @@
       </c>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B86" s="199" t="s">
+      <c r="B86" s="224" t="s">
         <v>59</v>
       </c>
-      <c r="C86" s="197"/>
-      <c r="D86" s="198"/>
+      <c r="C86" s="222"/>
+      <c r="D86" s="223"/>
       <c r="E86" s="108">
         <v>85</v>
       </c>
@@ -9927,11 +9927,11 @@
       </c>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B87" s="187" t="s">
+      <c r="B87" s="212" t="s">
         <v>21</v>
       </c>
-      <c r="C87" s="188"/>
-      <c r="D87" s="189"/>
+      <c r="C87" s="213"/>
+      <c r="D87" s="214"/>
       <c r="E87" s="155">
         <f t="shared" ref="E87:N87" si="60">SUM(E82:E86)</f>
         <v>3805</v>
@@ -9974,11 +9974,11 @@
       </c>
     </row>
     <row r="88" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="190" t="s">
+      <c r="B88" s="215" t="s">
         <v>21</v>
       </c>
-      <c r="C88" s="191"/>
-      <c r="D88" s="192"/>
+      <c r="C88" s="216"/>
+      <c r="D88" s="217"/>
       <c r="E88" s="174">
         <f>E80+E87</f>
         <v>62753.759999999995</v>
@@ -10022,6 +10022,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B86:D86"/>
     <mergeCell ref="N4:N6"/>
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="D7:D79"/>
@@ -10038,15 +10047,6 @@
     <mergeCell ref="K4:K6"/>
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B86:D86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10079,19 +10079,19 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="229"/>
-      <c r="C2" s="230"/>
-      <c r="D2" s="230"/>
-      <c r="E2" s="230"/>
-      <c r="F2" s="230"/>
-      <c r="G2" s="230"/>
-      <c r="H2" s="230"/>
-      <c r="I2" s="230"/>
-      <c r="J2" s="230"/>
-      <c r="K2" s="230"/>
-      <c r="L2" s="230"/>
-      <c r="M2" s="230"/>
-      <c r="N2" s="231"/>
+      <c r="B2" s="227"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="228"/>
+      <c r="J2" s="228"/>
+      <c r="K2" s="228"/>
+      <c r="L2" s="228"/>
+      <c r="M2" s="228"/>
+      <c r="N2" s="229"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="111"/>
@@ -10109,31 +10109,31 @@
       <c r="N3" s="113"/>
     </row>
     <row r="4" spans="1:14" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="240" t="s">
+      <c r="B4" s="238" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="241" t="s">
+      <c r="C4" s="239" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="246" t="s">
+      <c r="D4" s="244" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="247"/>
-      <c r="F4" s="247"/>
-      <c r="G4" s="247"/>
-      <c r="H4" s="247"/>
-      <c r="I4" s="247"/>
-      <c r="J4" s="247"/>
-      <c r="K4" s="247"/>
-      <c r="L4" s="247"/>
-      <c r="M4" s="248"/>
-      <c r="N4" s="242" t="s">
+      <c r="E4" s="245"/>
+      <c r="F4" s="245"/>
+      <c r="G4" s="245"/>
+      <c r="H4" s="245"/>
+      <c r="I4" s="245"/>
+      <c r="J4" s="245"/>
+      <c r="K4" s="245"/>
+      <c r="L4" s="245"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="240" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="240"/>
-      <c r="C5" s="241"/>
+      <c r="B5" s="238"/>
+      <c r="C5" s="239"/>
       <c r="D5" s="3">
         <v>1</v>
       </c>
@@ -10164,25 +10164,25 @@
       <c r="M5" s="3">
         <v>10</v>
       </c>
-      <c r="N5" s="242"/>
+      <c r="N5" s="240"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="243" t="s">
+      <c r="B6" s="241" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="244"/>
-      <c r="D6" s="244"/>
-      <c r="E6" s="244"/>
-      <c r="F6" s="244"/>
-      <c r="G6" s="244"/>
-      <c r="H6" s="244"/>
-      <c r="I6" s="244"/>
-      <c r="J6" s="244"/>
-      <c r="K6" s="244"/>
-      <c r="L6" s="244"/>
-      <c r="M6" s="245"/>
-      <c r="N6" s="242"/>
+      <c r="C6" s="242"/>
+      <c r="D6" s="242"/>
+      <c r="E6" s="242"/>
+      <c r="F6" s="242"/>
+      <c r="G6" s="242"/>
+      <c r="H6" s="242"/>
+      <c r="I6" s="242"/>
+      <c r="J6" s="242"/>
+      <c r="K6" s="242"/>
+      <c r="L6" s="242"/>
+      <c r="M6" s="243"/>
+      <c r="N6" s="240"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
@@ -10320,42 +10320,42 @@
       <c r="K10" s="2"/>
     </row>
     <row r="12" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="232" t="s">
+      <c r="B12" s="230" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="232"/>
-      <c r="D12" s="232"/>
-      <c r="E12" s="232"/>
-      <c r="F12" s="232"/>
-      <c r="G12" s="232"/>
-      <c r="H12" s="232"/>
-      <c r="I12" s="232"/>
-      <c r="J12" s="232"/>
-      <c r="K12" s="232"/>
-      <c r="L12" s="232"/>
-      <c r="M12" s="232"/>
+      <c r="C12" s="230"/>
+      <c r="D12" s="230"/>
+      <c r="E12" s="230"/>
+      <c r="F12" s="230"/>
+      <c r="G12" s="230"/>
+      <c r="H12" s="230"/>
+      <c r="I12" s="230"/>
+      <c r="J12" s="230"/>
+      <c r="K12" s="230"/>
+      <c r="L12" s="230"/>
+      <c r="M12" s="230"/>
     </row>
     <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="233" t="s">
+      <c r="D13" s="231" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="234"/>
-      <c r="F13" s="234"/>
-      <c r="G13" s="234"/>
-      <c r="H13" s="234"/>
-      <c r="I13" s="234"/>
-      <c r="J13" s="234"/>
-      <c r="K13" s="234"/>
-      <c r="L13" s="234"/>
-      <c r="M13" s="235"/>
+      <c r="E13" s="232"/>
+      <c r="F13" s="232"/>
+      <c r="G13" s="232"/>
+      <c r="H13" s="232"/>
+      <c r="I13" s="232"/>
+      <c r="J13" s="232"/>
+      <c r="K13" s="232"/>
+      <c r="L13" s="232"/>
+      <c r="M13" s="233"/>
     </row>
     <row r="14" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="236" t="s">
+      <c r="B14" s="234" t="s">
         <v>190</v>
       </c>
-      <c r="C14" s="237"/>
+      <c r="C14" s="235"/>
       <c r="D14" s="157">
         <v>1</v>
       </c>
@@ -10388,10 +10388,10 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="238" t="s">
+      <c r="B15" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="C15" s="239"/>
+      <c r="C15" s="237"/>
       <c r="D15" s="159">
         <v>3712.65</v>
       </c>
@@ -10424,10 +10424,10 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="226" t="s">
+      <c r="B16" s="225" t="s">
         <v>192</v>
       </c>
-      <c r="C16" s="227"/>
+      <c r="C16" s="226"/>
       <c r="D16" s="159">
         <v>3124.34</v>
       </c>
@@ -10460,10 +10460,10 @@
       </c>
     </row>
     <row r="17" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="226" t="s">
+      <c r="B17" s="225" t="s">
         <v>193</v>
       </c>
-      <c r="C17" s="227"/>
+      <c r="C17" s="226"/>
       <c r="D17" s="159">
         <v>2661.66</v>
       </c>
@@ -10496,10 +10496,10 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="226" t="s">
+      <c r="B18" s="225" t="s">
         <v>194</v>
       </c>
-      <c r="C18" s="227"/>
+      <c r="C18" s="226"/>
       <c r="D18" s="159">
         <v>3679.74</v>
       </c>
@@ -10532,10 +10532,10 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="226" t="s">
+      <c r="B19" s="225" t="s">
         <v>195</v>
       </c>
-      <c r="C19" s="227"/>
+      <c r="C19" s="226"/>
       <c r="D19" s="159">
         <v>7910.93</v>
       </c>
@@ -10568,10 +10568,10 @@
       </c>
     </row>
     <row r="20" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="226" t="s">
+      <c r="B20" s="225" t="s">
         <v>196</v>
       </c>
-      <c r="C20" s="227"/>
+      <c r="C20" s="226"/>
       <c r="D20" s="159">
         <v>6632.24</v>
       </c>
@@ -10604,10 +10604,10 @@
       </c>
     </row>
     <row r="21" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="226" t="s">
+      <c r="B21" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="C21" s="227"/>
+      <c r="C21" s="226"/>
       <c r="D21" s="159">
         <v>8738.19</v>
       </c>
@@ -10640,10 +10640,10 @@
       </c>
     </row>
     <row r="22" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="226" t="s">
+      <c r="B22" s="225" t="s">
         <v>198</v>
       </c>
-      <c r="C22" s="227"/>
+      <c r="C22" s="226"/>
       <c r="D22" s="159">
         <v>15266</v>
       </c>
@@ -10676,10 +10676,10 @@
       </c>
     </row>
     <row r="23" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="226" t="s">
+      <c r="B23" s="225" t="s">
         <v>199</v>
       </c>
-      <c r="C23" s="227"/>
+      <c r="C23" s="226"/>
       <c r="D23" s="159">
         <v>14281.22</v>
       </c>
@@ -10712,10 +10712,10 @@
       </c>
     </row>
     <row r="24" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="226" t="s">
+      <c r="B24" s="225" t="s">
         <v>200</v>
       </c>
-      <c r="C24" s="227"/>
+      <c r="C24" s="226"/>
       <c r="D24" s="159">
         <v>14897.24</v>
       </c>
@@ -10748,10 +10748,10 @@
       </c>
     </row>
     <row r="25" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="226" t="s">
+      <c r="B25" s="225" t="s">
         <v>201</v>
       </c>
-      <c r="C25" s="227"/>
+      <c r="C25" s="226"/>
       <c r="D25" s="159">
         <v>16082.55</v>
       </c>
@@ -10784,10 +10784,10 @@
       </c>
     </row>
     <row r="26" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="226" t="s">
+      <c r="B26" s="225" t="s">
         <v>202</v>
       </c>
-      <c r="C26" s="227"/>
+      <c r="C26" s="226"/>
       <c r="D26" s="159">
         <v>16284.26</v>
       </c>
@@ -10820,10 +10820,10 @@
       </c>
     </row>
     <row r="27" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="228" t="s">
+      <c r="B27" s="248" t="s">
         <v>203</v>
       </c>
-      <c r="C27" s="228"/>
+      <c r="C27" s="248"/>
       <c r="D27" s="167">
         <f t="shared" ref="D27:M27" si="1">SUM(D15:D26)</f>
         <v>113271.02</v>
@@ -10866,8 +10866,8 @@
       </c>
     </row>
     <row r="28" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="225"/>
-      <c r="C28" s="225"/>
+      <c r="B28" s="247"/>
+      <c r="C28" s="247"/>
       <c r="D28" s="112"/>
       <c r="E28" s="112"/>
       <c r="F28" s="112"/>
@@ -10880,8 +10880,8 @@
       <c r="M28" s="112"/>
     </row>
     <row r="29" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="225"/>
-      <c r="C29" s="225"/>
+      <c r="B29" s="247"/>
+      <c r="C29" s="247"/>
       <c r="D29" s="112"/>
       <c r="E29" s="112"/>
       <c r="F29" s="112"/>
@@ -10894,8 +10894,8 @@
       <c r="M29" s="112"/>
     </row>
     <row r="30" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="225"/>
-      <c r="C30" s="225"/>
+      <c r="B30" s="247"/>
+      <c r="C30" s="247"/>
       <c r="D30" s="112"/>
       <c r="E30" s="112"/>
       <c r="F30" s="112"/>
@@ -10908,8 +10908,8 @@
       <c r="M30" s="112"/>
     </row>
     <row r="31" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="225"/>
-      <c r="C31" s="225"/>
+      <c r="B31" s="247"/>
+      <c r="C31" s="247"/>
       <c r="D31" s="112"/>
       <c r="E31" s="112"/>
       <c r="F31" s="112"/>
@@ -10922,8 +10922,8 @@
       <c r="M31" s="112"/>
     </row>
     <row r="32" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="225"/>
-      <c r="C32" s="225"/>
+      <c r="B32" s="247"/>
+      <c r="C32" s="247"/>
       <c r="D32" s="112"/>
       <c r="E32" s="112"/>
       <c r="F32" s="112"/>
@@ -10983,14 +10983,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B12:M12"/>
     <mergeCell ref="D13:M13"/>
@@ -11001,15 +11002,14 @@
     <mergeCell ref="N4:N6"/>
     <mergeCell ref="B6:M6"/>
     <mergeCell ref="D4:M4"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -11062,15 +11062,15 @@
       <c r="C3" s="251" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="204"/>
-      <c r="E3" s="204"/>
-      <c r="F3" s="204"/>
-      <c r="G3" s="204"/>
-      <c r="H3" s="204"/>
-      <c r="I3" s="204"/>
-      <c r="J3" s="204"/>
-      <c r="K3" s="204"/>
-      <c r="L3" s="206"/>
+      <c r="D3" s="191"/>
+      <c r="E3" s="191"/>
+      <c r="F3" s="191"/>
+      <c r="G3" s="191"/>
+      <c r="H3" s="191"/>
+      <c r="I3" s="191"/>
+      <c r="J3" s="191"/>
+      <c r="K3" s="191"/>
+      <c r="L3" s="193"/>
       <c r="M3" s="135"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11430,8 +11430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AE64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="77" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="77" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11448,20 +11448,20 @@
   <sheetData>
     <row r="1" spans="2:31" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:31" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="263" t="s">
+      <c r="B2" s="267" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="264"/>
-      <c r="D2" s="264"/>
-      <c r="E2" s="264"/>
-      <c r="F2" s="264"/>
-      <c r="G2" s="264"/>
-      <c r="H2" s="264"/>
-      <c r="I2" s="264"/>
-      <c r="J2" s="264"/>
-      <c r="K2" s="264"/>
-      <c r="L2" s="264"/>
-      <c r="M2" s="264"/>
+      <c r="C2" s="268"/>
+      <c r="D2" s="268"/>
+      <c r="E2" s="268"/>
+      <c r="F2" s="268"/>
+      <c r="G2" s="268"/>
+      <c r="H2" s="268"/>
+      <c r="I2" s="268"/>
+      <c r="J2" s="268"/>
+      <c r="K2" s="268"/>
+      <c r="L2" s="268"/>
+      <c r="M2" s="268"/>
     </row>
     <row r="3" spans="2:31" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:31" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -12303,8 +12303,8 @@
       <c r="N19" s="76"/>
       <c r="O19" s="76"/>
       <c r="P19" s="76"/>
-      <c r="Q19" s="265"/>
-      <c r="R19" s="265"/>
+      <c r="Q19" s="255"/>
+      <c r="R19" s="255"/>
       <c r="S19" s="76"/>
       <c r="T19" s="76"/>
       <c r="U19" s="76"/>
@@ -12330,14 +12330,14 @@
       </c>
       <c r="G20" s="31"/>
       <c r="H20" s="32"/>
-      <c r="K20" s="265" t="s">
+      <c r="K20" s="255" t="s">
         <v>235</v>
       </c>
-      <c r="L20" s="265"/>
+      <c r="L20" s="255"/>
       <c r="M20" s="76"/>
       <c r="N20" s="76"/>
       <c r="O20" s="76"/>
-      <c r="P20" s="265"/>
+      <c r="P20" s="255"/>
       <c r="Q20" s="76"/>
       <c r="R20" s="77"/>
       <c r="S20" s="76"/>
@@ -12362,7 +12362,7 @@
       <c r="M21" s="76"/>
       <c r="N21" s="76"/>
       <c r="O21" s="76"/>
-      <c r="P21" s="265"/>
+      <c r="P21" s="255"/>
       <c r="Q21" s="76"/>
       <c r="R21" s="77"/>
       <c r="S21" s="76"/>
@@ -12425,16 +12425,16 @@
       <c r="Z23" s="76"/>
     </row>
     <row r="24" spans="2:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="260" t="s">
+      <c r="B24" s="264" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="261"/>
-      <c r="D24" s="261"/>
-      <c r="E24" s="261"/>
-      <c r="F24" s="261"/>
-      <c r="G24" s="261"/>
-      <c r="H24" s="261"/>
-      <c r="I24" s="262"/>
+      <c r="C24" s="265"/>
+      <c r="D24" s="265"/>
+      <c r="E24" s="265"/>
+      <c r="F24" s="265"/>
+      <c r="G24" s="265"/>
+      <c r="H24" s="265"/>
+      <c r="I24" s="266"/>
       <c r="J24" s="33"/>
       <c r="K24" s="80"/>
       <c r="L24" s="80"/>
@@ -12533,26 +12533,26 @@
       <c r="Z27" s="76"/>
     </row>
     <row r="28" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="256" t="s">
+      <c r="B28" s="260" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="255">
+      <c r="C28" s="259">
         <f>($C$18+NPV($F$20,$D$18:$M$18))</f>
         <v>1198.1821956073409</v>
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="48"/>
-      <c r="F28" s="268" t="s">
+      <c r="F28" s="258" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="258">
+      <c r="G28" s="262">
         <f>IRR(C18:M18)</f>
         <v>0.43661319726386583</v>
       </c>
-      <c r="H28" s="267" t="s">
+      <c r="H28" s="257" t="s">
         <v>52</v>
       </c>
-      <c r="I28" s="267"/>
+      <c r="I28" s="257"/>
       <c r="J28" s="33"/>
       <c r="K28" s="33"/>
       <c r="L28" s="33"/>
@@ -12560,17 +12560,17 @@
       <c r="N28" s="33"/>
     </row>
     <row r="29" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="257"/>
-      <c r="C29" s="255"/>
+      <c r="B29" s="261"/>
+      <c r="C29" s="259"/>
       <c r="D29" s="33"/>
       <c r="E29" s="48"/>
-      <c r="F29" s="268"/>
-      <c r="G29" s="259"/>
-      <c r="H29" s="266" t="str">
+      <c r="F29" s="258"/>
+      <c r="G29" s="263"/>
+      <c r="H29" s="256" t="str">
         <f>IF(G28&gt;=F20,"Se acepta el proyecto","Se rechaza el proyecto")</f>
         <v>Se acepta el proyecto</v>
       </c>
-      <c r="I29" s="266"/>
+      <c r="I29" s="256"/>
       <c r="J29" s="33"/>
       <c r="K29" s="33"/>
       <c r="L29" s="33"/>
@@ -13183,17 +13183,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B2:M2"/>
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="P20:P21"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="K20:L20"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="H29:I29">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/Carlos1200/ProyectoFinalAEE into main"
This reverts commit b87e2254bdcf422bfd9761ab115048b4f101271c, reversing
changes made to feab5b5943ba2cb9bab50218ed1360cdd9423565.
</commit_message>
<xml_diff>
--- a/Cálculos del Proyecto de AEEE.xlsx
+++ b/Cálculos del Proyecto de AEEE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdavi\Desktop\Proyecto AEE\ProyectoFinalAEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277CB672-E48A-42A1-A531-D1F76E6A85FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3613AE9F-6F87-4E0E-B377-71CE08221977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11310" tabRatio="814" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -743,7 +743,7 @@
     <t>(-) Impuestos 9%</t>
   </si>
   <si>
-    <t xml:space="preserve">Que ondas mariella </t>
+    <t>Que ondas mariella</t>
   </si>
 </sst>
 </file>
@@ -2486,81 +2486,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="21" borderId="62" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="21" borderId="63" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="21" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2603,12 +2528,93 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="21" borderId="62" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="21" borderId="63" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="21" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2669,12 +2675,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2692,6 +2692,36 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="5" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="14" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="14" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2705,36 +2735,6 @@
     </xf>
     <xf numFmtId="169" fontId="13" fillId="15" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="5" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="13" fillId="14" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="13" fillId="14" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -6062,49 +6062,49 @@
   <sheetData>
     <row r="1" spans="2:14" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="194" t="s">
+      <c r="B2" s="207" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="195"/>
-      <c r="L2" s="195"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="196"/>
+      <c r="C2" s="208"/>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+      <c r="G2" s="208"/>
+      <c r="H2" s="208"/>
+      <c r="I2" s="208"/>
+      <c r="J2" s="208"/>
+      <c r="K2" s="208"/>
+      <c r="L2" s="208"/>
+      <c r="M2" s="208"/>
+      <c r="N2" s="209"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="210" t="s">
         <v>187</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="199"/>
-      <c r="E3" s="191" t="s">
+      <c r="C3" s="211"/>
+      <c r="D3" s="212"/>
+      <c r="E3" s="204" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="192"/>
-      <c r="G3" s="191"/>
-      <c r="H3" s="191"/>
-      <c r="I3" s="191"/>
-      <c r="J3" s="191"/>
-      <c r="K3" s="191"/>
-      <c r="L3" s="191"/>
-      <c r="M3" s="191"/>
-      <c r="N3" s="193"/>
+      <c r="F3" s="205"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="204"/>
+      <c r="J3" s="204"/>
+      <c r="K3" s="204"/>
+      <c r="L3" s="204"/>
+      <c r="M3" s="204"/>
+      <c r="N3" s="206"/>
     </row>
     <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="200"/>
-      <c r="C4" s="201"/>
-      <c r="D4" s="201"/>
-      <c r="E4" s="204">
+      <c r="B4" s="213"/>
+      <c r="C4" s="214"/>
+      <c r="D4" s="214"/>
+      <c r="E4" s="217">
         <v>1</v>
       </c>
-      <c r="F4" s="207">
+      <c r="F4" s="220">
         <v>2</v>
       </c>
       <c r="G4" s="184">
@@ -6133,15 +6133,15 @@
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="210" t="s">
+      <c r="B5" s="223" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="211"/>
-      <c r="D5" s="202" t="s">
+      <c r="C5" s="224"/>
+      <c r="D5" s="215" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="205"/>
-      <c r="F5" s="208"/>
+      <c r="E5" s="218"/>
+      <c r="F5" s="221"/>
       <c r="G5" s="185"/>
       <c r="H5" s="185"/>
       <c r="I5" s="185"/>
@@ -6158,9 +6158,9 @@
       <c r="C6" s="142" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="203"/>
-      <c r="E6" s="206"/>
-      <c r="F6" s="209"/>
+      <c r="D6" s="216"/>
+      <c r="E6" s="219"/>
+      <c r="F6" s="222"/>
       <c r="G6" s="186"/>
       <c r="H6" s="186"/>
       <c r="I6" s="186"/>
@@ -6177,7 +6177,7 @@
       <c r="C7" s="138" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="188">
+      <c r="D7" s="201">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E7" s="143">
@@ -6227,7 +6227,7 @@
       <c r="C8" s="138" t="s">
         <v>135</v>
       </c>
-      <c r="D8" s="189"/>
+      <c r="D8" s="202"/>
       <c r="E8" s="145">
         <v>56</v>
       </c>
@@ -6275,7 +6275,7 @@
       <c r="C9" s="138" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="189"/>
+      <c r="D9" s="202"/>
       <c r="E9" s="145">
         <v>84</v>
       </c>
@@ -6323,7 +6323,7 @@
       <c r="C10" s="138" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="189"/>
+      <c r="D10" s="202"/>
       <c r="E10" s="145">
         <v>23</v>
       </c>
@@ -6371,7 +6371,7 @@
       <c r="C11" s="138" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="189"/>
+      <c r="D11" s="202"/>
       <c r="E11" s="145">
         <v>16</v>
       </c>
@@ -6419,7 +6419,7 @@
       <c r="C12" s="138" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="189"/>
+      <c r="D12" s="202"/>
       <c r="E12" s="145">
         <v>14</v>
       </c>
@@ -6467,7 +6467,7 @@
       <c r="C13" s="138" t="s">
         <v>140</v>
       </c>
-      <c r="D13" s="189"/>
+      <c r="D13" s="202"/>
       <c r="E13" s="145">
         <v>35</v>
       </c>
@@ -6515,7 +6515,7 @@
       <c r="C14" s="138" t="s">
         <v>141</v>
       </c>
-      <c r="D14" s="189"/>
+      <c r="D14" s="202"/>
       <c r="E14" s="145">
         <v>14</v>
       </c>
@@ -6563,7 +6563,7 @@
       <c r="C15" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="D15" s="189"/>
+      <c r="D15" s="202"/>
       <c r="E15" s="145">
         <v>7.5</v>
       </c>
@@ -6611,7 +6611,7 @@
       <c r="C16" s="138" t="s">
         <v>143</v>
       </c>
-      <c r="D16" s="189"/>
+      <c r="D16" s="202"/>
       <c r="E16" s="145">
         <v>5</v>
       </c>
@@ -6659,7 +6659,7 @@
       <c r="C17" s="138" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="189"/>
+      <c r="D17" s="202"/>
       <c r="E17" s="145">
         <v>3.75</v>
       </c>
@@ -6707,7 +6707,7 @@
       <c r="C18" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="D18" s="189"/>
+      <c r="D18" s="202"/>
       <c r="E18" s="145">
         <v>10</v>
       </c>
@@ -6755,7 +6755,7 @@
       <c r="C19" s="138" t="s">
         <v>144</v>
       </c>
-      <c r="D19" s="189"/>
+      <c r="D19" s="202"/>
       <c r="E19" s="145">
         <v>28</v>
       </c>
@@ -6803,7 +6803,7 @@
       <c r="C20" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="D20" s="189"/>
+      <c r="D20" s="202"/>
       <c r="E20" s="145">
         <v>25</v>
       </c>
@@ -6851,7 +6851,7 @@
       <c r="C21" s="138" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="189"/>
+      <c r="D21" s="202"/>
       <c r="E21" s="145">
         <v>6.3</v>
       </c>
@@ -6899,7 +6899,7 @@
       <c r="C22" s="138" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="189"/>
+      <c r="D22" s="202"/>
       <c r="E22" s="145">
         <v>227.5</v>
       </c>
@@ -6947,7 +6947,7 @@
       <c r="C23" s="138" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="189"/>
+      <c r="D23" s="202"/>
       <c r="E23" s="145">
         <v>70</v>
       </c>
@@ -6995,7 +6995,7 @@
       <c r="C24" s="138" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="189"/>
+      <c r="D24" s="202"/>
       <c r="E24" s="145">
         <v>30.5</v>
       </c>
@@ -7043,7 +7043,7 @@
       <c r="C25" s="138" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="189"/>
+      <c r="D25" s="202"/>
       <c r="E25" s="145">
         <v>85.5</v>
       </c>
@@ -7091,7 +7091,7 @@
       <c r="C26" s="138" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="189"/>
+      <c r="D26" s="202"/>
       <c r="E26" s="145">
         <v>175</v>
       </c>
@@ -7139,7 +7139,7 @@
       <c r="C27" s="138" t="s">
         <v>148</v>
       </c>
-      <c r="D27" s="189"/>
+      <c r="D27" s="202"/>
       <c r="E27" s="145">
         <v>31.5</v>
       </c>
@@ -7187,7 +7187,7 @@
       <c r="C28" s="138" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="189"/>
+      <c r="D28" s="202"/>
       <c r="E28" s="147">
         <v>141.75</v>
       </c>
@@ -7235,7 +7235,7 @@
       <c r="C29" s="140" t="s">
         <v>146</v>
       </c>
-      <c r="D29" s="189"/>
+      <c r="D29" s="202"/>
       <c r="E29" s="147">
         <v>80.5</v>
       </c>
@@ -7283,7 +7283,7 @@
       <c r="C30" s="140" t="s">
         <v>152</v>
       </c>
-      <c r="D30" s="189"/>
+      <c r="D30" s="202"/>
       <c r="E30" s="147">
         <f>702/52</f>
         <v>13.5</v>
@@ -7332,7 +7332,7 @@
       <c r="C31" s="140" t="s">
         <v>153</v>
       </c>
-      <c r="D31" s="189"/>
+      <c r="D31" s="202"/>
       <c r="E31" s="147">
         <v>28.56</v>
       </c>
@@ -7380,7 +7380,7 @@
       <c r="C32" s="140" t="s">
         <v>154</v>
       </c>
-      <c r="D32" s="189"/>
+      <c r="D32" s="202"/>
       <c r="E32" s="147">
         <v>7</v>
       </c>
@@ -7428,7 +7428,7 @@
       <c r="C33" s="140" t="s">
         <v>155</v>
       </c>
-      <c r="D33" s="189"/>
+      <c r="D33" s="202"/>
       <c r="E33" s="147">
         <v>15</v>
       </c>
@@ -7476,7 +7476,7 @@
       <c r="C34" s="140" t="s">
         <v>156</v>
       </c>
-      <c r="D34" s="189"/>
+      <c r="D34" s="202"/>
       <c r="E34" s="147">
         <v>20.58</v>
       </c>
@@ -7524,7 +7524,7 @@
       <c r="C35" s="140" t="s">
         <v>157</v>
       </c>
-      <c r="D35" s="189"/>
+      <c r="D35" s="202"/>
       <c r="E35" s="147">
         <v>22.72</v>
       </c>
@@ -7572,7 +7572,7 @@
       <c r="C36" s="140" t="s">
         <v>158</v>
       </c>
-      <c r="D36" s="189"/>
+      <c r="D36" s="202"/>
       <c r="E36" s="147">
         <v>8</v>
       </c>
@@ -7620,7 +7620,7 @@
       <c r="C37" s="140" t="s">
         <v>158</v>
       </c>
-      <c r="D37" s="189"/>
+      <c r="D37" s="202"/>
       <c r="E37" s="147">
         <v>8</v>
       </c>
@@ -7668,7 +7668,7 @@
       <c r="C38" s="140" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="189"/>
+      <c r="D38" s="202"/>
       <c r="E38" s="147">
         <v>11.25</v>
       </c>
@@ -7716,7 +7716,7 @@
       <c r="C39" s="140" t="s">
         <v>159</v>
       </c>
-      <c r="D39" s="189"/>
+      <c r="D39" s="202"/>
       <c r="E39" s="147">
         <v>12.5</v>
       </c>
@@ -7764,7 +7764,7 @@
       <c r="C40" s="140" t="s">
         <v>160</v>
       </c>
-      <c r="D40" s="189"/>
+      <c r="D40" s="202"/>
       <c r="E40" s="147">
         <v>12</v>
       </c>
@@ -7812,7 +7812,7 @@
       <c r="C41" s="140" t="s">
         <v>143</v>
       </c>
-      <c r="D41" s="189"/>
+      <c r="D41" s="202"/>
       <c r="E41" s="147">
         <v>10</v>
       </c>
@@ -7860,7 +7860,7 @@
       <c r="C42" s="140" t="s">
         <v>161</v>
       </c>
-      <c r="D42" s="189"/>
+      <c r="D42" s="202"/>
       <c r="E42" s="147">
         <v>120</v>
       </c>
@@ -7908,7 +7908,7 @@
       <c r="C43" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D43" s="189"/>
+      <c r="D43" s="202"/>
       <c r="E43" s="147">
         <v>66</v>
       </c>
@@ -7956,7 +7956,7 @@
       <c r="C44" s="140" t="s">
         <v>163</v>
       </c>
-      <c r="D44" s="189"/>
+      <c r="D44" s="202"/>
       <c r="E44" s="147">
         <v>7</v>
       </c>
@@ -8004,7 +8004,7 @@
       <c r="C45" s="140" t="s">
         <v>178</v>
       </c>
-      <c r="D45" s="189"/>
+      <c r="D45" s="202"/>
       <c r="E45" s="147">
         <v>2.72</v>
       </c>
@@ -8052,7 +8052,7 @@
       <c r="C46" s="140" t="s">
         <v>164</v>
       </c>
-      <c r="D46" s="189"/>
+      <c r="D46" s="202"/>
       <c r="E46" s="147">
         <v>3.6</v>
       </c>
@@ -8100,7 +8100,7 @@
       <c r="C47" s="140" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="189"/>
+      <c r="D47" s="202"/>
       <c r="E47" s="147">
         <v>4.25</v>
       </c>
@@ -8148,7 +8148,7 @@
       <c r="C48" s="140" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="189"/>
+      <c r="D48" s="202"/>
       <c r="E48" s="147">
         <v>4.25</v>
       </c>
@@ -8196,7 +8196,7 @@
       <c r="C49" s="140" t="s">
         <v>166</v>
       </c>
-      <c r="D49" s="189"/>
+      <c r="D49" s="202"/>
       <c r="E49" s="147">
         <v>6</v>
       </c>
@@ -8244,7 +8244,7 @@
       <c r="C50" s="140" t="s">
         <v>164</v>
       </c>
-      <c r="D50" s="189"/>
+      <c r="D50" s="202"/>
       <c r="E50" s="147">
         <v>9</v>
       </c>
@@ -8292,7 +8292,7 @@
       <c r="C51" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="D51" s="189"/>
+      <c r="D51" s="202"/>
       <c r="E51" s="147">
         <v>7</v>
       </c>
@@ -8340,7 +8340,7 @@
       <c r="C52" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="D52" s="189"/>
+      <c r="D52" s="202"/>
       <c r="E52" s="147">
         <v>8</v>
       </c>
@@ -8388,7 +8388,7 @@
       <c r="C53" s="140" t="s">
         <v>148</v>
       </c>
-      <c r="D53" s="189"/>
+      <c r="D53" s="202"/>
       <c r="E53" s="147">
         <v>10</v>
       </c>
@@ -8436,7 +8436,7 @@
       <c r="C54" s="140" t="s">
         <v>168</v>
       </c>
-      <c r="D54" s="189"/>
+      <c r="D54" s="202"/>
       <c r="E54" s="147">
         <v>4.9000000000000004</v>
       </c>
@@ -8484,7 +8484,7 @@
       <c r="C55" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="D55" s="189"/>
+      <c r="D55" s="202"/>
       <c r="E55" s="147">
         <v>18</v>
       </c>
@@ -8532,7 +8532,7 @@
       <c r="C56" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="D56" s="189"/>
+      <c r="D56" s="202"/>
       <c r="E56" s="147">
         <v>10</v>
       </c>
@@ -8580,7 +8580,7 @@
       <c r="C57" s="140" t="s">
         <v>171</v>
       </c>
-      <c r="D57" s="189"/>
+      <c r="D57" s="202"/>
       <c r="E57" s="147">
         <v>7</v>
       </c>
@@ -8628,7 +8628,7 @@
       <c r="C58" s="140" t="s">
         <v>172</v>
       </c>
-      <c r="D58" s="189"/>
+      <c r="D58" s="202"/>
       <c r="E58" s="147">
         <v>1.58</v>
       </c>
@@ -8676,7 +8676,7 @@
       <c r="C59" s="140" t="s">
         <v>173</v>
       </c>
-      <c r="D59" s="189"/>
+      <c r="D59" s="202"/>
       <c r="E59" s="147">
         <v>19</v>
       </c>
@@ -8724,7 +8724,7 @@
       <c r="C60" s="140" t="s">
         <v>174</v>
       </c>
-      <c r="D60" s="189"/>
+      <c r="D60" s="202"/>
       <c r="E60" s="147">
         <v>5.4</v>
       </c>
@@ -8772,7 +8772,7 @@
       <c r="C61" s="140" t="s">
         <v>175</v>
       </c>
-      <c r="D61" s="189"/>
+      <c r="D61" s="202"/>
       <c r="E61" s="147">
         <v>6.25</v>
       </c>
@@ -8820,7 +8820,7 @@
       <c r="C62" s="140" t="s">
         <v>176</v>
       </c>
-      <c r="D62" s="189"/>
+      <c r="D62" s="202"/>
       <c r="E62" s="147">
         <v>4.5</v>
       </c>
@@ -8868,7 +8868,7 @@
       <c r="C63" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="D63" s="189"/>
+      <c r="D63" s="202"/>
       <c r="E63" s="149">
         <v>42</v>
       </c>
@@ -8916,7 +8916,7 @@
       <c r="C64" s="140" t="s">
         <v>211</v>
       </c>
-      <c r="D64" s="189"/>
+      <c r="D64" s="202"/>
       <c r="E64" s="166">
         <v>15.2</v>
       </c>
@@ -8964,7 +8964,7 @@
       <c r="C65" s="140" t="s">
         <v>212</v>
       </c>
-      <c r="D65" s="189"/>
+      <c r="D65" s="202"/>
       <c r="E65" s="166">
         <v>6.96</v>
       </c>
@@ -9012,7 +9012,7 @@
       <c r="C66" s="140" t="s">
         <v>213</v>
       </c>
-      <c r="D66" s="189"/>
+      <c r="D66" s="202"/>
       <c r="E66" s="166">
         <v>16.32</v>
       </c>
@@ -9060,7 +9060,7 @@
       <c r="C67" s="140" t="s">
         <v>213</v>
       </c>
-      <c r="D67" s="189"/>
+      <c r="D67" s="202"/>
       <c r="E67" s="166">
         <v>16.32</v>
       </c>
@@ -9108,7 +9108,7 @@
       <c r="C68" s="140" t="s">
         <v>214</v>
       </c>
-      <c r="D68" s="189"/>
+      <c r="D68" s="202"/>
       <c r="E68" s="166">
         <v>5.5</v>
       </c>
@@ -9156,7 +9156,7 @@
       <c r="C69" s="140" t="s">
         <v>215</v>
       </c>
-      <c r="D69" s="189"/>
+      <c r="D69" s="202"/>
       <c r="E69" s="166">
         <v>13</v>
       </c>
@@ -9204,7 +9204,7 @@
       <c r="C70" s="140" t="s">
         <v>216</v>
       </c>
-      <c r="D70" s="189"/>
+      <c r="D70" s="202"/>
       <c r="E70" s="166">
         <v>141.12</v>
       </c>
@@ -9252,7 +9252,7 @@
       <c r="C71" s="140" t="s">
         <v>217</v>
       </c>
-      <c r="D71" s="189"/>
+      <c r="D71" s="202"/>
       <c r="E71" s="166">
         <v>15.68</v>
       </c>
@@ -9300,7 +9300,7 @@
       <c r="C72" s="140" t="s">
         <v>226</v>
       </c>
-      <c r="D72" s="189"/>
+      <c r="D72" s="202"/>
       <c r="E72" s="165">
         <v>54.6</v>
       </c>
@@ -9348,7 +9348,7 @@
       <c r="C73" s="140" t="s">
         <v>227</v>
       </c>
-      <c r="D73" s="189"/>
+      <c r="D73" s="202"/>
       <c r="E73" s="165">
         <v>11</v>
       </c>
@@ -9396,7 +9396,7 @@
       <c r="C74" s="140" t="s">
         <v>228</v>
       </c>
-      <c r="D74" s="189"/>
+      <c r="D74" s="202"/>
       <c r="E74" s="165">
         <v>56.1</v>
       </c>
@@ -9444,7 +9444,7 @@
       <c r="C75" s="140" t="s">
         <v>229</v>
       </c>
-      <c r="D75" s="189"/>
+      <c r="D75" s="202"/>
       <c r="E75" s="165">
         <v>15</v>
       </c>
@@ -9492,7 +9492,7 @@
       <c r="C76" s="140" t="s">
         <v>230</v>
       </c>
-      <c r="D76" s="189"/>
+      <c r="D76" s="202"/>
       <c r="E76" s="165">
         <v>90</v>
       </c>
@@ -9540,7 +9540,7 @@
       <c r="C77" s="140" t="s">
         <v>231</v>
       </c>
-      <c r="D77" s="189"/>
+      <c r="D77" s="202"/>
       <c r="E77" s="165">
         <v>4</v>
       </c>
@@ -9588,7 +9588,7 @@
       <c r="C78" s="140" t="s">
         <v>232</v>
       </c>
-      <c r="D78" s="189"/>
+      <c r="D78" s="202"/>
       <c r="E78" s="165">
         <v>4.0999999999999996</v>
       </c>
@@ -9636,7 +9636,7 @@
       <c r="C79" s="140" t="s">
         <v>233</v>
       </c>
-      <c r="D79" s="190"/>
+      <c r="D79" s="203"/>
       <c r="E79" s="165">
         <v>7</v>
       </c>
@@ -9678,10 +9678,10 @@
       </c>
     </row>
     <row r="80" spans="2:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="187" t="s">
+      <c r="B80" s="200" t="s">
         <v>188</v>
       </c>
-      <c r="C80" s="187"/>
+      <c r="C80" s="200"/>
       <c r="D80" s="176"/>
       <c r="E80" s="171">
         <f>SUM(E7:E79)*26</f>
@@ -9725,11 +9725,11 @@
       </c>
     </row>
     <row r="81" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="218" t="s">
+      <c r="B81" s="193" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="219"/>
-      <c r="D81" s="220"/>
+      <c r="C81" s="194"/>
+      <c r="D81" s="195"/>
       <c r="E81" s="172"/>
       <c r="F81" s="172"/>
       <c r="G81" s="172"/>
@@ -9742,11 +9742,11 @@
       <c r="N81" s="173"/>
     </row>
     <row r="82" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="221" t="s">
+      <c r="B82" s="196" t="s">
         <v>67</v>
       </c>
-      <c r="C82" s="222"/>
-      <c r="D82" s="223"/>
+      <c r="C82" s="197"/>
+      <c r="D82" s="198"/>
       <c r="E82" s="108">
         <v>300</v>
       </c>
@@ -9779,11 +9779,11 @@
       </c>
     </row>
     <row r="83" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="221" t="s">
+      <c r="B83" s="196" t="s">
         <v>68</v>
       </c>
-      <c r="C83" s="222"/>
-      <c r="D83" s="223"/>
+      <c r="C83" s="197"/>
+      <c r="D83" s="198"/>
       <c r="E83" s="108">
         <v>1100</v>
       </c>
@@ -9816,11 +9816,11 @@
       </c>
     </row>
     <row r="84" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="221" t="s">
+      <c r="B84" s="196" t="s">
         <v>69</v>
       </c>
-      <c r="C84" s="222"/>
-      <c r="D84" s="223"/>
+      <c r="C84" s="197"/>
+      <c r="D84" s="198"/>
       <c r="E84" s="108">
         <v>400</v>
       </c>
@@ -9853,11 +9853,11 @@
       </c>
     </row>
     <row r="85" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="221" t="s">
+      <c r="B85" s="196" t="s">
         <v>185</v>
       </c>
-      <c r="C85" s="222"/>
-      <c r="D85" s="223"/>
+      <c r="C85" s="197"/>
+      <c r="D85" s="198"/>
       <c r="E85" s="108">
         <v>1920</v>
       </c>
@@ -9890,11 +9890,11 @@
       </c>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B86" s="224" t="s">
+      <c r="B86" s="199" t="s">
         <v>59</v>
       </c>
-      <c r="C86" s="222"/>
-      <c r="D86" s="223"/>
+      <c r="C86" s="197"/>
+      <c r="D86" s="198"/>
       <c r="E86" s="108">
         <v>85</v>
       </c>
@@ -9927,11 +9927,11 @@
       </c>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B87" s="212" t="s">
+      <c r="B87" s="187" t="s">
         <v>21</v>
       </c>
-      <c r="C87" s="213"/>
-      <c r="D87" s="214"/>
+      <c r="C87" s="188"/>
+      <c r="D87" s="189"/>
       <c r="E87" s="155">
         <f t="shared" ref="E87:N87" si="60">SUM(E82:E86)</f>
         <v>3805</v>
@@ -9974,11 +9974,11 @@
       </c>
     </row>
     <row r="88" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="215" t="s">
+      <c r="B88" s="190" t="s">
         <v>21</v>
       </c>
-      <c r="C88" s="216"/>
-      <c r="D88" s="217"/>
+      <c r="C88" s="191"/>
+      <c r="D88" s="192"/>
       <c r="E88" s="174">
         <f>E80+E87</f>
         <v>62753.759999999995</v>
@@ -10022,15 +10022,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B86:D86"/>
     <mergeCell ref="N4:N6"/>
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="D7:D79"/>
@@ -10047,6 +10038,15 @@
     <mergeCell ref="K4:K6"/>
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B86:D86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10079,19 +10079,19 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="227"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
-      <c r="L2" s="228"/>
-      <c r="M2" s="228"/>
-      <c r="N2" s="229"/>
+      <c r="B2" s="229"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
+      <c r="L2" s="230"/>
+      <c r="M2" s="230"/>
+      <c r="N2" s="231"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="111"/>
@@ -10109,31 +10109,31 @@
       <c r="N3" s="113"/>
     </row>
     <row r="4" spans="1:14" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="238" t="s">
+      <c r="B4" s="240" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="239" t="s">
+      <c r="C4" s="241" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="244" t="s">
+      <c r="D4" s="246" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="245"/>
-      <c r="F4" s="245"/>
-      <c r="G4" s="245"/>
-      <c r="H4" s="245"/>
-      <c r="I4" s="245"/>
-      <c r="J4" s="245"/>
-      <c r="K4" s="245"/>
-      <c r="L4" s="245"/>
-      <c r="M4" s="246"/>
-      <c r="N4" s="240" t="s">
+      <c r="E4" s="247"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
+      <c r="L4" s="247"/>
+      <c r="M4" s="248"/>
+      <c r="N4" s="242" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="238"/>
-      <c r="C5" s="239"/>
+      <c r="B5" s="240"/>
+      <c r="C5" s="241"/>
       <c r="D5" s="3">
         <v>1</v>
       </c>
@@ -10164,25 +10164,25 @@
       <c r="M5" s="3">
         <v>10</v>
       </c>
-      <c r="N5" s="240"/>
+      <c r="N5" s="242"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="241" t="s">
+      <c r="B6" s="243" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="242"/>
-      <c r="D6" s="242"/>
-      <c r="E6" s="242"/>
-      <c r="F6" s="242"/>
-      <c r="G6" s="242"/>
-      <c r="H6" s="242"/>
-      <c r="I6" s="242"/>
-      <c r="J6" s="242"/>
-      <c r="K6" s="242"/>
-      <c r="L6" s="242"/>
-      <c r="M6" s="243"/>
-      <c r="N6" s="240"/>
+      <c r="C6" s="244"/>
+      <c r="D6" s="244"/>
+      <c r="E6" s="244"/>
+      <c r="F6" s="244"/>
+      <c r="G6" s="244"/>
+      <c r="H6" s="244"/>
+      <c r="I6" s="244"/>
+      <c r="J6" s="244"/>
+      <c r="K6" s="244"/>
+      <c r="L6" s="244"/>
+      <c r="M6" s="245"/>
+      <c r="N6" s="242"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
@@ -10320,42 +10320,42 @@
       <c r="K10" s="2"/>
     </row>
     <row r="12" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="230" t="s">
+      <c r="B12" s="232" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="230"/>
-      <c r="D12" s="230"/>
-      <c r="E12" s="230"/>
-      <c r="F12" s="230"/>
-      <c r="G12" s="230"/>
-      <c r="H12" s="230"/>
-      <c r="I12" s="230"/>
-      <c r="J12" s="230"/>
-      <c r="K12" s="230"/>
-      <c r="L12" s="230"/>
-      <c r="M12" s="230"/>
+      <c r="C12" s="232"/>
+      <c r="D12" s="232"/>
+      <c r="E12" s="232"/>
+      <c r="F12" s="232"/>
+      <c r="G12" s="232"/>
+      <c r="H12" s="232"/>
+      <c r="I12" s="232"/>
+      <c r="J12" s="232"/>
+      <c r="K12" s="232"/>
+      <c r="L12" s="232"/>
+      <c r="M12" s="232"/>
     </row>
     <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="231" t="s">
+      <c r="D13" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="232"/>
-      <c r="F13" s="232"/>
-      <c r="G13" s="232"/>
-      <c r="H13" s="232"/>
-      <c r="I13" s="232"/>
-      <c r="J13" s="232"/>
-      <c r="K13" s="232"/>
-      <c r="L13" s="232"/>
-      <c r="M13" s="233"/>
+      <c r="E13" s="234"/>
+      <c r="F13" s="234"/>
+      <c r="G13" s="234"/>
+      <c r="H13" s="234"/>
+      <c r="I13" s="234"/>
+      <c r="J13" s="234"/>
+      <c r="K13" s="234"/>
+      <c r="L13" s="234"/>
+      <c r="M13" s="235"/>
     </row>
     <row r="14" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="234" t="s">
+      <c r="B14" s="236" t="s">
         <v>190</v>
       </c>
-      <c r="C14" s="235"/>
+      <c r="C14" s="237"/>
       <c r="D14" s="157">
         <v>1</v>
       </c>
@@ -10388,10 +10388,10 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="236" t="s">
+      <c r="B15" s="238" t="s">
         <v>191</v>
       </c>
-      <c r="C15" s="237"/>
+      <c r="C15" s="239"/>
       <c r="D15" s="159">
         <v>3712.65</v>
       </c>
@@ -10424,10 +10424,10 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="225" t="s">
+      <c r="B16" s="226" t="s">
         <v>192</v>
       </c>
-      <c r="C16" s="226"/>
+      <c r="C16" s="227"/>
       <c r="D16" s="159">
         <v>3124.34</v>
       </c>
@@ -10460,10 +10460,10 @@
       </c>
     </row>
     <row r="17" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="225" t="s">
+      <c r="B17" s="226" t="s">
         <v>193</v>
       </c>
-      <c r="C17" s="226"/>
+      <c r="C17" s="227"/>
       <c r="D17" s="159">
         <v>2661.66</v>
       </c>
@@ -10496,10 +10496,10 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="225" t="s">
+      <c r="B18" s="226" t="s">
         <v>194</v>
       </c>
-      <c r="C18" s="226"/>
+      <c r="C18" s="227"/>
       <c r="D18" s="159">
         <v>3679.74</v>
       </c>
@@ -10532,10 +10532,10 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="225" t="s">
+      <c r="B19" s="226" t="s">
         <v>195</v>
       </c>
-      <c r="C19" s="226"/>
+      <c r="C19" s="227"/>
       <c r="D19" s="159">
         <v>7910.93</v>
       </c>
@@ -10568,10 +10568,10 @@
       </c>
     </row>
     <row r="20" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="225" t="s">
+      <c r="B20" s="226" t="s">
         <v>196</v>
       </c>
-      <c r="C20" s="226"/>
+      <c r="C20" s="227"/>
       <c r="D20" s="159">
         <v>6632.24</v>
       </c>
@@ -10604,10 +10604,10 @@
       </c>
     </row>
     <row r="21" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="225" t="s">
+      <c r="B21" s="226" t="s">
         <v>197</v>
       </c>
-      <c r="C21" s="226"/>
+      <c r="C21" s="227"/>
       <c r="D21" s="159">
         <v>8738.19</v>
       </c>
@@ -10640,10 +10640,10 @@
       </c>
     </row>
     <row r="22" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="225" t="s">
+      <c r="B22" s="226" t="s">
         <v>198</v>
       </c>
-      <c r="C22" s="226"/>
+      <c r="C22" s="227"/>
       <c r="D22" s="159">
         <v>15266</v>
       </c>
@@ -10676,10 +10676,10 @@
       </c>
     </row>
     <row r="23" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="225" t="s">
+      <c r="B23" s="226" t="s">
         <v>199</v>
       </c>
-      <c r="C23" s="226"/>
+      <c r="C23" s="227"/>
       <c r="D23" s="159">
         <v>14281.22</v>
       </c>
@@ -10712,10 +10712,10 @@
       </c>
     </row>
     <row r="24" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="225" t="s">
+      <c r="B24" s="226" t="s">
         <v>200</v>
       </c>
-      <c r="C24" s="226"/>
+      <c r="C24" s="227"/>
       <c r="D24" s="159">
         <v>14897.24</v>
       </c>
@@ -10748,10 +10748,10 @@
       </c>
     </row>
     <row r="25" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="225" t="s">
+      <c r="B25" s="226" t="s">
         <v>201</v>
       </c>
-      <c r="C25" s="226"/>
+      <c r="C25" s="227"/>
       <c r="D25" s="159">
         <v>16082.55</v>
       </c>
@@ -10784,10 +10784,10 @@
       </c>
     </row>
     <row r="26" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="225" t="s">
+      <c r="B26" s="226" t="s">
         <v>202</v>
       </c>
-      <c r="C26" s="226"/>
+      <c r="C26" s="227"/>
       <c r="D26" s="159">
         <v>16284.26</v>
       </c>
@@ -10820,10 +10820,10 @@
       </c>
     </row>
     <row r="27" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="248" t="s">
+      <c r="B27" s="228" t="s">
         <v>203</v>
       </c>
-      <c r="C27" s="248"/>
+      <c r="C27" s="228"/>
       <c r="D27" s="167">
         <f t="shared" ref="D27:M27" si="1">SUM(D15:D26)</f>
         <v>113271.02</v>
@@ -10866,8 +10866,8 @@
       </c>
     </row>
     <row r="28" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="247"/>
-      <c r="C28" s="247"/>
+      <c r="B28" s="225"/>
+      <c r="C28" s="225"/>
       <c r="D28" s="112"/>
       <c r="E28" s="112"/>
       <c r="F28" s="112"/>
@@ -10880,8 +10880,8 @@
       <c r="M28" s="112"/>
     </row>
     <row r="29" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="247"/>
-      <c r="C29" s="247"/>
+      <c r="B29" s="225"/>
+      <c r="C29" s="225"/>
       <c r="D29" s="112"/>
       <c r="E29" s="112"/>
       <c r="F29" s="112"/>
@@ -10894,8 +10894,8 @@
       <c r="M29" s="112"/>
     </row>
     <row r="30" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="247"/>
-      <c r="C30" s="247"/>
+      <c r="B30" s="225"/>
+      <c r="C30" s="225"/>
       <c r="D30" s="112"/>
       <c r="E30" s="112"/>
       <c r="F30" s="112"/>
@@ -10908,8 +10908,8 @@
       <c r="M30" s="112"/>
     </row>
     <row r="31" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="247"/>
-      <c r="C31" s="247"/>
+      <c r="B31" s="225"/>
+      <c r="C31" s="225"/>
       <c r="D31" s="112"/>
       <c r="E31" s="112"/>
       <c r="F31" s="112"/>
@@ -10922,8 +10922,8 @@
       <c r="M31" s="112"/>
     </row>
     <row r="32" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="247"/>
-      <c r="C32" s="247"/>
+      <c r="B32" s="225"/>
+      <c r="C32" s="225"/>
       <c r="D32" s="112"/>
       <c r="E32" s="112"/>
       <c r="F32" s="112"/>
@@ -10983,15 +10983,14 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B12:M12"/>
     <mergeCell ref="D13:M13"/>
@@ -11002,14 +11001,15 @@
     <mergeCell ref="N4:N6"/>
     <mergeCell ref="B6:M6"/>
     <mergeCell ref="D4:M4"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -11062,15 +11062,15 @@
       <c r="C3" s="251" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="191"/>
-      <c r="E3" s="191"/>
-      <c r="F3" s="191"/>
-      <c r="G3" s="191"/>
-      <c r="H3" s="191"/>
-      <c r="I3" s="191"/>
-      <c r="J3" s="191"/>
-      <c r="K3" s="191"/>
-      <c r="L3" s="193"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="204"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="204"/>
+      <c r="J3" s="204"/>
+      <c r="K3" s="204"/>
+      <c r="L3" s="206"/>
       <c r="M3" s="135"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11430,8 +11430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AE64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="77" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="77" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11448,20 +11448,20 @@
   <sheetData>
     <row r="1" spans="2:31" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:31" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="267" t="s">
+      <c r="B2" s="263" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="268"/>
-      <c r="D2" s="268"/>
-      <c r="E2" s="268"/>
-      <c r="F2" s="268"/>
-      <c r="G2" s="268"/>
-      <c r="H2" s="268"/>
-      <c r="I2" s="268"/>
-      <c r="J2" s="268"/>
-      <c r="K2" s="268"/>
-      <c r="L2" s="268"/>
-      <c r="M2" s="268"/>
+      <c r="C2" s="264"/>
+      <c r="D2" s="264"/>
+      <c r="E2" s="264"/>
+      <c r="F2" s="264"/>
+      <c r="G2" s="264"/>
+      <c r="H2" s="264"/>
+      <c r="I2" s="264"/>
+      <c r="J2" s="264"/>
+      <c r="K2" s="264"/>
+      <c r="L2" s="264"/>
+      <c r="M2" s="264"/>
     </row>
     <row r="3" spans="2:31" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:31" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -12303,8 +12303,8 @@
       <c r="N19" s="76"/>
       <c r="O19" s="76"/>
       <c r="P19" s="76"/>
-      <c r="Q19" s="255"/>
-      <c r="R19" s="255"/>
+      <c r="Q19" s="265"/>
+      <c r="R19" s="265"/>
       <c r="S19" s="76"/>
       <c r="T19" s="76"/>
       <c r="U19" s="76"/>
@@ -12330,14 +12330,14 @@
       </c>
       <c r="G20" s="31"/>
       <c r="H20" s="32"/>
-      <c r="K20" s="255" t="s">
+      <c r="K20" s="265" t="s">
         <v>235</v>
       </c>
-      <c r="L20" s="255"/>
+      <c r="L20" s="265"/>
       <c r="M20" s="76"/>
       <c r="N20" s="76"/>
       <c r="O20" s="76"/>
-      <c r="P20" s="255"/>
+      <c r="P20" s="265"/>
       <c r="Q20" s="76"/>
       <c r="R20" s="77"/>
       <c r="S20" s="76"/>
@@ -12362,7 +12362,7 @@
       <c r="M21" s="76"/>
       <c r="N21" s="76"/>
       <c r="O21" s="76"/>
-      <c r="P21" s="255"/>
+      <c r="P21" s="265"/>
       <c r="Q21" s="76"/>
       <c r="R21" s="77"/>
       <c r="S21" s="76"/>
@@ -12425,16 +12425,16 @@
       <c r="Z23" s="76"/>
     </row>
     <row r="24" spans="2:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="264" t="s">
+      <c r="B24" s="260" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="265"/>
-      <c r="D24" s="265"/>
-      <c r="E24" s="265"/>
-      <c r="F24" s="265"/>
-      <c r="G24" s="265"/>
-      <c r="H24" s="265"/>
-      <c r="I24" s="266"/>
+      <c r="C24" s="261"/>
+      <c r="D24" s="261"/>
+      <c r="E24" s="261"/>
+      <c r="F24" s="261"/>
+      <c r="G24" s="261"/>
+      <c r="H24" s="261"/>
+      <c r="I24" s="262"/>
       <c r="J24" s="33"/>
       <c r="K24" s="80"/>
       <c r="L24" s="80"/>
@@ -12533,26 +12533,26 @@
       <c r="Z27" s="76"/>
     </row>
     <row r="28" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="260" t="s">
+      <c r="B28" s="256" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="259">
+      <c r="C28" s="255">
         <f>($C$18+NPV($F$20,$D$18:$M$18))</f>
         <v>1198.1821956073409</v>
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="48"/>
-      <c r="F28" s="258" t="s">
+      <c r="F28" s="268" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="262">
+      <c r="G28" s="258">
         <f>IRR(C18:M18)</f>
         <v>0.43661319726386583</v>
       </c>
-      <c r="H28" s="257" t="s">
+      <c r="H28" s="267" t="s">
         <v>52</v>
       </c>
-      <c r="I28" s="257"/>
+      <c r="I28" s="267"/>
       <c r="J28" s="33"/>
       <c r="K28" s="33"/>
       <c r="L28" s="33"/>
@@ -12560,17 +12560,17 @@
       <c r="N28" s="33"/>
     </row>
     <row r="29" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="261"/>
-      <c r="C29" s="259"/>
+      <c r="B29" s="257"/>
+      <c r="C29" s="255"/>
       <c r="D29" s="33"/>
       <c r="E29" s="48"/>
-      <c r="F29" s="258"/>
-      <c r="G29" s="263"/>
-      <c r="H29" s="256" t="str">
+      <c r="F29" s="268"/>
+      <c r="G29" s="259"/>
+      <c r="H29" s="266" t="str">
         <f>IF(G28&gt;=F20,"Se acepta el proyecto","Se rechaza el proyecto")</f>
         <v>Se acepta el proyecto</v>
       </c>
-      <c r="I29" s="256"/>
+      <c r="I29" s="266"/>
       <c r="J29" s="33"/>
       <c r="K29" s="33"/>
       <c r="L29" s="33"/>
@@ -13183,17 +13183,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B2:M2"/>
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="P20:P21"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="K20:L20"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="H29:I29">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>